<commit_message>
Update bat/sh scripts for new DSB definitions.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo_new_antisense.xlsx
+++ b/analyze_nhej/libinfo_new_antisense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB41A636-5996-4134-A13E-C014CFB6DFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E45DB47-3CD2-43A9-81CC-3AE2DFC5E057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -886,6 +886,15 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -992,12 +1001,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2052,9 +2055,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -2110,50 +2110,50 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="115">
   <autoFilter ref="A1:O41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="15">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="113"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="112">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="113">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="111">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="112">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="110">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="111">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="109">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="110">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="108">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="109">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="107">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="108">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="106">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="107">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="105">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="106">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="104">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="105">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="103">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="104">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="102">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="103">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="101">
+    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="102">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="100">
+    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="101">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="99">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="100">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2166,46 +2166,46 @@
   <autoFilter ref="A43:O55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="98">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="99">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="97">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="98">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="96">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="97">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="95">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="96">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="94">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="95">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="93">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="94">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="92">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="93">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="91">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="92">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="90">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="91">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="89">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="90">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="88">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="89">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="87">
+    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="88">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="86">
+    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="87">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="85">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="86">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2214,36 +2214,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="85">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="83"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="82">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="84"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="83">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="81">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="82">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="80">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="81">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="79">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="80">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="78">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="79">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="77">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="78">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="76">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="77">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2252,32 +2252,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="76">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="74"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="73">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="75"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="74">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="72">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="73">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="71">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="72">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="70">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="71">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="69">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="70">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="68">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="69">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="67">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="68">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2286,36 +2286,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="63">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="64">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="62">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="63">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="61">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="62">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="60">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="61">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="59">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="60">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="58">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="59">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="57">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="58">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2324,44 +2324,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AB42" totalsRowShown="0" headerRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AB42" totalsRowShown="0" headerRowDxfId="57">
   <autoFilter ref="A2:AB42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="28">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="55"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="54">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="55">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="53">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="54">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="52">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="53">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="51">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="52">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="50">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="51">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="49">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="50">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="49">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="48">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="45">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="43">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="44">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2373,45 +2373,45 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="43">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="41">
+    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="42">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -12, IF(table_7_1[[#This Row],[hguide]]="CD", -12, IF(table_7_1[[#This Row],[hguide]]="A", -12, IF(table_7_1[[#This Row],[hguide]]="B", -12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="40">
+    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="41">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 13, IF(table_7_1[[#This Row],[hguide]]="CD", 13, IF(table_7_1[[#This Row],[hguide]]="A", 13, IF(table_7_1[[#This Row],[hguide]]="B", 13, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="39">
-      <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</calculatedColumnFormula>
+    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="0">
+      <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{FCD7272B-07C5-4D80-8B2B-EFDF0948D1A3}" name="range_y1" dataDxfId="38">
+    <tableColumn id="18" xr3:uid="{FCD7272B-07C5-4D80-8B2B-EFDF0948D1A3}" name="range_y1" dataDxfId="40">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 22, IF(table_7_1[[#This Row],[hguide]]="CD", 27, IF(table_7_1[[#This Row],[hguide]]="A", 20, IF(table_7_1[[#This Row],[hguide]]="B", 16, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="37">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="39">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT("--range_x ", table_7_1[[#This Row],[range_x0]], " ", table_7_1[[#This Row],[range_x1]], " --range_y ", table_7_1[[#This Row],[range_y0]], " ", table_7_1[[#This Row],[range_y1]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{862E4B1D-E776-4C82-956F-64077E0EAD63}" name="universal_layout_y_axis_args" dataDxfId="36">
+    <tableColumn id="29" xr3:uid="{862E4B1D-E776-4C82-956F-64077E0EAD63}" name="universal_layout_y_axis_args" dataDxfId="38">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_x_pos ", table_7_1[[#This Row],[range_x1]] - 1, " --universal_layout_y_axis_y_range ", table_7_1[[#This Row],[range_y0]] + 2.5, " ", table_7_1[[#This Row],[range_y1]] - 1.5, " "), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{80C9383B-6A26-4051-B986-65C11BA3AFE0}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="23" xr3:uid="{010D8635-D593-4849-BEA6-27994308E467}" name="universal_layout_x_axis_args" dataDxfId="35">
+    <tableColumn id="23" xr3:uid="{010D8635-D593-4849-BEA6-27994308E467}" name="universal_layout_x_axis_args" dataDxfId="37">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[show_universal_layout_x_axes]], _xlfn.CONCAT(" --universal_layout_x_axis_deletion_y_pos ", table_7_1[[#This Row],[range_y0]] + 1.5, " --universal_layout_x_axis_insertion_y_pos ", table_7_1[[#This Row],[range_y1]] - 0.5, " --universal_layout_x_axis_x_range ", table_7_1[[#This Row],[range_x0]] + 0.5, " ", table_7_1[[#This Row],[range_x1]] - 1.5), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="34">
+    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="36">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 7, IF(table_7_1[[#This Row],[hguide]]="CD", 8, IF(table_7_1[[#This Row],[hguide]]="A", 6, IF(table_7_1[[#This Row],[hguide]]="B", 5, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="33">
-      <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="1">
+      <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="32">
+    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="35">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="31">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="34">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{C5B2A575-6AC4-403E-AE67-1624B7F60F7E}" name="format"/>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="30">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="33">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2420,46 +2420,46 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="A44:O60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="30">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="29">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="28">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="24">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="23">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="22">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="20">
+    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{EADBB7DC-9D40-44C2-8742-A17A0EB899C3}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="19">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="22">
       <calculatedColumnFormula>IF(table_7_2[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="18">
+    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="17">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="20">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{8B58B2DF-3EB7-4D4E-A96D-1BED892121E3}" name="format"/>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="16">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2468,46 +2468,46 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A62:O64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="16">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="7">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="6">
+    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="4">
+    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="7">
       <calculatedColumnFormula>IF(table_7_3[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="3">
+    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="6">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2527,25 +2527,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="214">
-      <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="2">
+      <calculatedColumnFormula array="1">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="213">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="214">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="212">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="213">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="211">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="212">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="210">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="211">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="209">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="210">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="208">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="209">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2554,38 +2554,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="207">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="208">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="206"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="205">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="207"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="206">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="204">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="205">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="203">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="204">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="202">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="203">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="201">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="202">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="200">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="201">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="199">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="200">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="198">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="199">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="197">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="198">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="196">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="197">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2597,19 +2597,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="195">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="196">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="194">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="195">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="193">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="194">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="192">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="193">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="191">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="192">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2621,41 +2621,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="190"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="189">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="191"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="190">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="188">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="187">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="186">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="185">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="184">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="183">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="182">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="181">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="182">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="180">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="181">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="179">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="180">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="178">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="179">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2664,47 +2664,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="178">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="176"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="175">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="177"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="176">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="174">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="175">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="173">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="174">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="172">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="171">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="170">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="171">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="169">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="168">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="169">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="167">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="166">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="165">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="166">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="164">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="165">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2713,47 +2713,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="164">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="162"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="161">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="163"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="162">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="160">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="159">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="160">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="158">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="159">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="157">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="156">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="157">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="155">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="156">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="154">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="155">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="153">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="154">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="152">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="151">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="152">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="150">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="151">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2762,38 +2762,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="150">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="148"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="147">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="149"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="148">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="146">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="147">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="145">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="146">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="144">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="145">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="143">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="142">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="143">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="141">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="142">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="140">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="141">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="139">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="140">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="138">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="139">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2802,38 +2802,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="138">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="135">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="137"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="136">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="134">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="135">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="133">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="134">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="132">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="133">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="131">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="132">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="130">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="131">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="129">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="130">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="128">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="129">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="127">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="128">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2842,38 +2842,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="127">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="125"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="124">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="126"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="125">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="123">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="124">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="122">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="123">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="121">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="122">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="120">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="121">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="119">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="120">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="118">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="119">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="117">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="118">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="116">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="117">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="115">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="116">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5007,8 +5007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158:XFD161"/>
+    <sheetView topLeftCell="B163" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5102,7 +5102,7 @@
         <v>83</v>
       </c>
       <c r="I2" cm="1">
-        <f t="array" ref="I2">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I2">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J2" t="str">
@@ -5156,7 +5156,7 @@
         <v>83</v>
       </c>
       <c r="I3" cm="1">
-        <f t="array" ref="I3">IF(E3="2DSB", IF(H3="R1", 67, 46), IF(E3="1DSB", IF(H3="R1", 67, 46), IF(E3="2DSBanti", IF(H3="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I3">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J3" t="str">
@@ -5210,7 +5210,7 @@
         <v>83</v>
       </c>
       <c r="I4" cm="1">
-        <f t="array" ref="I4">IF(E4="2DSB", IF(H4="R1", 67, 46), IF(E4="1DSB", IF(H4="R1", 67, 46), IF(E4="2DSBanti", IF(H4="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I4">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J4" t="str">
@@ -5264,7 +5264,7 @@
         <v>83</v>
       </c>
       <c r="I5" cm="1">
-        <f t="array" ref="I5">IF(E5="2DSB", IF(H5="R1", 67, 46), IF(E5="1DSB", IF(H5="R1", 67, 46), IF(E5="2DSBanti", IF(H5="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I5">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J5" t="str">
@@ -5318,7 +5318,7 @@
         <v>83</v>
       </c>
       <c r="I6" cm="1">
-        <f t="array" ref="I6">IF(E6="2DSB", IF(H6="R1", 67, 46), IF(E6="1DSB", IF(H6="R1", 67, 46), IF(E6="2DSBanti", IF(H6="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I6">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J6" t="str">
@@ -5372,7 +5372,7 @@
         <v>83</v>
       </c>
       <c r="I7" cm="1">
-        <f t="array" ref="I7">IF(E7="2DSB", IF(H7="R1", 67, 46), IF(E7="1DSB", IF(H7="R1", 67, 46), IF(E7="2DSBanti", IF(H7="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I7">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J7" t="str">
@@ -5426,7 +5426,7 @@
         <v>83</v>
       </c>
       <c r="I8" cm="1">
-        <f t="array" ref="I8">IF(E8="2DSB", IF(H8="R1", 67, 46), IF(E8="1DSB", IF(H8="R1", 67, 46), IF(E8="2DSBanti", IF(H8="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I8">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J8" t="str">
@@ -5480,7 +5480,7 @@
         <v>83</v>
       </c>
       <c r="I9" cm="1">
-        <f t="array" ref="I9">IF(E9="2DSB", IF(H9="R1", 67, 46), IF(E9="1DSB", IF(H9="R1", 67, 46), IF(E9="2DSBanti", IF(H9="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I9">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J9" t="str">
@@ -5534,7 +5534,7 @@
         <v>83</v>
       </c>
       <c r="I10" cm="1">
-        <f t="array" ref="I10">IF(E10="2DSB", IF(H10="R1", 67, 46), IF(E10="1DSB", IF(H10="R1", 67, 46), IF(E10="2DSBanti", IF(H10="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I10">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J10" t="str">
@@ -5588,7 +5588,7 @@
         <v>83</v>
       </c>
       <c r="I11" cm="1">
-        <f t="array" ref="I11">IF(E11="2DSB", IF(H11="R1", 67, 46), IF(E11="1DSB", IF(H11="R1", 67, 46), IF(E11="2DSBanti", IF(H11="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I11">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J11" t="str">
@@ -5642,7 +5642,7 @@
         <v>83</v>
       </c>
       <c r="I12" cm="1">
-        <f t="array" ref="I12">IF(E12="2DSB", IF(H12="R1", 67, 46), IF(E12="1DSB", IF(H12="R1", 67, 46), IF(E12="2DSBanti", IF(H12="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I12">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J12" t="str">
@@ -5696,7 +5696,7 @@
         <v>83</v>
       </c>
       <c r="I13" cm="1">
-        <f t="array" ref="I13">IF(E13="2DSB", IF(H13="R1", 67, 46), IF(E13="1DSB", IF(H13="R1", 67, 46), IF(E13="2DSBanti", IF(H13="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I13">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J13" t="str">
@@ -5750,7 +5750,7 @@
         <v>83</v>
       </c>
       <c r="I14" cm="1">
-        <f t="array" ref="I14">IF(E14="2DSB", IF(H14="R1", 67, 46), IF(E14="1DSB", IF(H14="R1", 67, 46), IF(E14="2DSBanti", IF(H14="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I14">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J14" t="str">
@@ -5804,7 +5804,7 @@
         <v>83</v>
       </c>
       <c r="I15" cm="1">
-        <f t="array" ref="I15">IF(E15="2DSB", IF(H15="R1", 67, 46), IF(E15="1DSB", IF(H15="R1", 67, 46), IF(E15="2DSBanti", IF(H15="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I15">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J15" t="str">
@@ -5858,7 +5858,7 @@
         <v>83</v>
       </c>
       <c r="I16" cm="1">
-        <f t="array" ref="I16">IF(E16="2DSB", IF(H16="R1", 67, 46), IF(E16="1DSB", IF(H16="R1", 67, 46), IF(E16="2DSBanti", IF(H16="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I16">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J16" t="str">
@@ -5912,7 +5912,7 @@
         <v>83</v>
       </c>
       <c r="I17" cm="1">
-        <f t="array" ref="I17">IF(E17="2DSB", IF(H17="R1", 67, 46), IF(E17="1DSB", IF(H17="R1", 67, 46), IF(E17="2DSBanti", IF(H17="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I17">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J17" t="str">
@@ -5966,7 +5966,7 @@
         <v>83</v>
       </c>
       <c r="I18" cm="1">
-        <f t="array" ref="I18">IF(E18="2DSB", IF(H18="R1", 67, 46), IF(E18="1DSB", IF(H18="R1", 67, 46), IF(E18="2DSBanti", IF(H18="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I18">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J18" t="str">
@@ -6020,7 +6020,7 @@
         <v>83</v>
       </c>
       <c r="I19" cm="1">
-        <f t="array" ref="I19">IF(E19="2DSB", IF(H19="R1", 67, 46), IF(E19="1DSB", IF(H19="R1", 67, 46), IF(E19="2DSBanti", IF(H19="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I19">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J19" t="str">
@@ -6074,7 +6074,7 @@
         <v>83</v>
       </c>
       <c r="I20" cm="1">
-        <f t="array" ref="I20">IF(E20="2DSB", IF(H20="R1", 67, 46), IF(E20="1DSB", IF(H20="R1", 67, 46), IF(E20="2DSBanti", IF(H20="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I20">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J20" t="str">
@@ -6128,7 +6128,7 @@
         <v>83</v>
       </c>
       <c r="I21" cm="1">
-        <f t="array" ref="I21">IF(E21="2DSB", IF(H21="R1", 67, 46), IF(E21="1DSB", IF(H21="R1", 67, 46), IF(E21="2DSBanti", IF(H21="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I21">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J21" t="str">
@@ -6182,7 +6182,7 @@
         <v>83</v>
       </c>
       <c r="I22" cm="1">
-        <f t="array" ref="I22">IF(E22="2DSB", IF(H22="R1", 67, 46), IF(E22="1DSB", IF(H22="R1", 67, 46), IF(E22="2DSBanti", IF(H22="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I22">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J22" t="str">
@@ -6236,7 +6236,7 @@
         <v>83</v>
       </c>
       <c r="I23" cm="1">
-        <f t="array" ref="I23">IF(E23="2DSB", IF(H23="R1", 67, 46), IF(E23="1DSB", IF(H23="R1", 67, 46), IF(E23="2DSBanti", IF(H23="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I23">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J23" t="str">
@@ -6290,7 +6290,7 @@
         <v>83</v>
       </c>
       <c r="I24" cm="1">
-        <f t="array" ref="I24">IF(E24="2DSB", IF(H24="R1", 67, 46), IF(E24="1DSB", IF(H24="R1", 67, 46), IF(E24="2DSBanti", IF(H24="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I24">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J24" t="str">
@@ -6344,7 +6344,7 @@
         <v>83</v>
       </c>
       <c r="I25" cm="1">
-        <f t="array" ref="I25">IF(E25="2DSB", IF(H25="R1", 67, 46), IF(E25="1DSB", IF(H25="R1", 67, 46), IF(E25="2DSBanti", IF(H25="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I25">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J25" t="str">
@@ -6398,7 +6398,7 @@
         <v>84</v>
       </c>
       <c r="I26" cm="1">
-        <f t="array" ref="I26">IF(E26="2DSB", IF(H26="R1", 67, 46), IF(E26="1DSB", IF(H26="R1", 67, 46), IF(E26="2DSBanti", IF(H26="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I26">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J26" t="str">
@@ -6452,7 +6452,7 @@
         <v>84</v>
       </c>
       <c r="I27" cm="1">
-        <f t="array" ref="I27">IF(E27="2DSB", IF(H27="R1", 67, 46), IF(E27="1DSB", IF(H27="R1", 67, 46), IF(E27="2DSBanti", IF(H27="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I27">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J27" t="str">
@@ -6506,7 +6506,7 @@
         <v>84</v>
       </c>
       <c r="I28" cm="1">
-        <f t="array" ref="I28">IF(E28="2DSB", IF(H28="R1", 67, 46), IF(E28="1DSB", IF(H28="R1", 67, 46), IF(E28="2DSBanti", IF(H28="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I28">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J28" t="str">
@@ -6560,7 +6560,7 @@
         <v>84</v>
       </c>
       <c r="I29" cm="1">
-        <f t="array" ref="I29">IF(E29="2DSB", IF(H29="R1", 67, 46), IF(E29="1DSB", IF(H29="R1", 67, 46), IF(E29="2DSBanti", IF(H29="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I29">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J29" t="str">
@@ -6614,7 +6614,7 @@
         <v>84</v>
       </c>
       <c r="I30" cm="1">
-        <f t="array" ref="I30">IF(E30="2DSB", IF(H30="R1", 67, 46), IF(E30="1DSB", IF(H30="R1", 67, 46), IF(E30="2DSBanti", IF(H30="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I30">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J30" t="str">
@@ -6668,7 +6668,7 @@
         <v>84</v>
       </c>
       <c r="I31" cm="1">
-        <f t="array" ref="I31">IF(E31="2DSB", IF(H31="R1", 67, 46), IF(E31="1DSB", IF(H31="R1", 67, 46), IF(E31="2DSBanti", IF(H31="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I31">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J31" t="str">
@@ -6722,7 +6722,7 @@
         <v>84</v>
       </c>
       <c r="I32" cm="1">
-        <f t="array" ref="I32">IF(E32="2DSB", IF(H32="R1", 67, 46), IF(E32="1DSB", IF(H32="R1", 67, 46), IF(E32="2DSBanti", IF(H32="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I32">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J32" t="str">
@@ -6776,7 +6776,7 @@
         <v>84</v>
       </c>
       <c r="I33" cm="1">
-        <f t="array" ref="I33">IF(E33="2DSB", IF(H33="R1", 67, 46), IF(E33="1DSB", IF(H33="R1", 67, 46), IF(E33="2DSBanti", IF(H33="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I33">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J33" t="str">
@@ -6830,7 +6830,7 @@
         <v>84</v>
       </c>
       <c r="I34" cm="1">
-        <f t="array" ref="I34">IF(E34="2DSB", IF(H34="R1", 67, 46), IF(E34="1DSB", IF(H34="R1", 67, 46), IF(E34="2DSBanti", IF(H34="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I34">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J34" t="str">
@@ -6884,7 +6884,7 @@
         <v>84</v>
       </c>
       <c r="I35" cm="1">
-        <f t="array" ref="I35">IF(E35="2DSB", IF(H35="R1", 67, 46), IF(E35="1DSB", IF(H35="R1", 67, 46), IF(E35="2DSBanti", IF(H35="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I35">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J35" t="str">
@@ -6938,7 +6938,7 @@
         <v>84</v>
       </c>
       <c r="I36" cm="1">
-        <f t="array" ref="I36">IF(E36="2DSB", IF(H36="R1", 67, 46), IF(E36="1DSB", IF(H36="R1", 67, 46), IF(E36="2DSBanti", IF(H36="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I36">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J36" t="str">
@@ -6992,7 +6992,7 @@
         <v>84</v>
       </c>
       <c r="I37" cm="1">
-        <f t="array" ref="I37">IF(E37="2DSB", IF(H37="R1", 67, 46), IF(E37="1DSB", IF(H37="R1", 67, 46), IF(E37="2DSBanti", IF(H37="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I37">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J37" t="str">
@@ -7046,7 +7046,7 @@
         <v>84</v>
       </c>
       <c r="I38" cm="1">
-        <f t="array" ref="I38">IF(E38="2DSB", IF(H38="R1", 67, 46), IF(E38="1DSB", IF(H38="R1", 67, 46), IF(E38="2DSBanti", IF(H38="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I38">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J38" t="str">
@@ -7100,7 +7100,7 @@
         <v>84</v>
       </c>
       <c r="I39" cm="1">
-        <f t="array" ref="I39">IF(E39="2DSB", IF(H39="R1", 67, 46), IF(E39="1DSB", IF(H39="R1", 67, 46), IF(E39="2DSBanti", IF(H39="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I39">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J39" t="str">
@@ -7154,7 +7154,7 @@
         <v>84</v>
       </c>
       <c r="I40" cm="1">
-        <f t="array" ref="I40">IF(E40="2DSB", IF(H40="R1", 67, 46), IF(E40="1DSB", IF(H40="R1", 67, 46), IF(E40="2DSBanti", IF(H40="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I40">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J40" t="str">
@@ -7208,7 +7208,7 @@
         <v>84</v>
       </c>
       <c r="I41" cm="1">
-        <f t="array" ref="I41">IF(E41="2DSB", IF(H41="R1", 67, 46), IF(E41="1DSB", IF(H41="R1", 67, 46), IF(E41="2DSBanti", IF(H41="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I41">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J41" t="str">
@@ -7262,7 +7262,7 @@
         <v>84</v>
       </c>
       <c r="I42" cm="1">
-        <f t="array" ref="I42">IF(E42="2DSB", IF(H42="R1", 67, 46), IF(E42="1DSB", IF(H42="R1", 67, 46), IF(E42="2DSBanti", IF(H42="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I42">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J42" t="str">
@@ -7316,7 +7316,7 @@
         <v>84</v>
       </c>
       <c r="I43" cm="1">
-        <f t="array" ref="I43">IF(E43="2DSB", IF(H43="R1", 67, 46), IF(E43="1DSB", IF(H43="R1", 67, 46), IF(E43="2DSBanti", IF(H43="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I43">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J43" t="str">
@@ -7370,7 +7370,7 @@
         <v>84</v>
       </c>
       <c r="I44" cm="1">
-        <f t="array" ref="I44">IF(E44="2DSB", IF(H44="R1", 67, 46), IF(E44="1DSB", IF(H44="R1", 67, 46), IF(E44="2DSBanti", IF(H44="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I44">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J44" t="str">
@@ -7424,7 +7424,7 @@
         <v>84</v>
       </c>
       <c r="I45" cm="1">
-        <f t="array" ref="I45">IF(E45="2DSB", IF(H45="R1", 67, 46), IF(E45="1DSB", IF(H45="R1", 67, 46), IF(E45="2DSBanti", IF(H45="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I45">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J45" t="str">
@@ -7478,7 +7478,7 @@
         <v>84</v>
       </c>
       <c r="I46" cm="1">
-        <f t="array" ref="I46">IF(E46="2DSB", IF(H46="R1", 67, 46), IF(E46="1DSB", IF(H46="R1", 67, 46), IF(E46="2DSBanti", IF(H46="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I46">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J46" t="str">
@@ -7532,7 +7532,7 @@
         <v>84</v>
       </c>
       <c r="I47" cm="1">
-        <f t="array" ref="I47">IF(E47="2DSB", IF(H47="R1", 67, 46), IF(E47="1DSB", IF(H47="R1", 67, 46), IF(E47="2DSBanti", IF(H47="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I47">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J47" t="str">
@@ -7586,7 +7586,7 @@
         <v>84</v>
       </c>
       <c r="I48" cm="1">
-        <f t="array" ref="I48">IF(E48="2DSB", IF(H48="R1", 67, 46), IF(E48="1DSB", IF(H48="R1", 67, 46), IF(E48="2DSBanti", IF(H48="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I48">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J48" t="str">
@@ -7640,7 +7640,7 @@
         <v>84</v>
       </c>
       <c r="I49" cm="1">
-        <f t="array" ref="I49">IF(E49="2DSB", IF(H49="R1", 67, 46), IF(E49="1DSB", IF(H49="R1", 67, 46), IF(E49="2DSBanti", IF(H49="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I49">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J49" t="str">
@@ -7694,7 +7694,7 @@
         <v>83</v>
       </c>
       <c r="I50" cm="1">
-        <f t="array" ref="I50">IF(E50="2DSB", IF(H50="R1", 67, 46), IF(E50="1DSB", IF(H50="R1", 67, 46), IF(E50="2DSBanti", IF(H50="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I50">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J50" t="str">
@@ -7748,7 +7748,7 @@
         <v>83</v>
       </c>
       <c r="I51" cm="1">
-        <f t="array" ref="I51">IF(E51="2DSB", IF(H51="R1", 67, 46), IF(E51="1DSB", IF(H51="R1", 67, 46), IF(E51="2DSBanti", IF(H51="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I51">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J51" t="str">
@@ -7802,7 +7802,7 @@
         <v>83</v>
       </c>
       <c r="I52" cm="1">
-        <f t="array" ref="I52">IF(E52="2DSB", IF(H52="R1", 67, 46), IF(E52="1DSB", IF(H52="R1", 67, 46), IF(E52="2DSBanti", IF(H52="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I52">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J52" t="str">
@@ -7856,7 +7856,7 @@
         <v>83</v>
       </c>
       <c r="I53" cm="1">
-        <f t="array" ref="I53">IF(E53="2DSB", IF(H53="R1", 67, 46), IF(E53="1DSB", IF(H53="R1", 67, 46), IF(E53="2DSBanti", IF(H53="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I53">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J53" t="str">
@@ -7910,7 +7910,7 @@
         <v>83</v>
       </c>
       <c r="I54" cm="1">
-        <f t="array" ref="I54">IF(E54="2DSB", IF(H54="R1", 67, 46), IF(E54="1DSB", IF(H54="R1", 67, 46), IF(E54="2DSBanti", IF(H54="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I54">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J54" t="str">
@@ -7964,7 +7964,7 @@
         <v>83</v>
       </c>
       <c r="I55" cm="1">
-        <f t="array" ref="I55">IF(E55="2DSB", IF(H55="R1", 67, 46), IF(E55="1DSB", IF(H55="R1", 67, 46), IF(E55="2DSBanti", IF(H55="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I55">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J55" t="str">
@@ -8018,7 +8018,7 @@
         <v>83</v>
       </c>
       <c r="I56" cm="1">
-        <f t="array" ref="I56">IF(E56="2DSB", IF(H56="R1", 67, 46), IF(E56="1DSB", IF(H56="R1", 67, 46), IF(E56="2DSBanti", IF(H56="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I56">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J56" t="str">
@@ -8072,7 +8072,7 @@
         <v>83</v>
       </c>
       <c r="I57" cm="1">
-        <f t="array" ref="I57">IF(E57="2DSB", IF(H57="R1", 67, 46), IF(E57="1DSB", IF(H57="R1", 67, 46), IF(E57="2DSBanti", IF(H57="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I57">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J57" t="str">
@@ -8126,7 +8126,7 @@
         <v>83</v>
       </c>
       <c r="I58" cm="1">
-        <f t="array" ref="I58">IF(E58="2DSB", IF(H58="R1", 67, 46), IF(E58="1DSB", IF(H58="R1", 67, 46), IF(E58="2DSBanti", IF(H58="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I58">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J58" t="str">
@@ -8180,7 +8180,7 @@
         <v>83</v>
       </c>
       <c r="I59" cm="1">
-        <f t="array" ref="I59">IF(E59="2DSB", IF(H59="R1", 67, 46), IF(E59="1DSB", IF(H59="R1", 67, 46), IF(E59="2DSBanti", IF(H59="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I59">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J59" t="str">
@@ -8234,7 +8234,7 @@
         <v>83</v>
       </c>
       <c r="I60" cm="1">
-        <f t="array" ref="I60">IF(E60="2DSB", IF(H60="R1", 67, 46), IF(E60="1DSB", IF(H60="R1", 67, 46), IF(E60="2DSBanti", IF(H60="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I60">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J60" t="str">
@@ -8288,7 +8288,7 @@
         <v>83</v>
       </c>
       <c r="I61" cm="1">
-        <f t="array" ref="I61">IF(E61="2DSB", IF(H61="R1", 67, 46), IF(E61="1DSB", IF(H61="R1", 67, 46), IF(E61="2DSBanti", IF(H61="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I61">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J61" t="str">
@@ -8342,7 +8342,7 @@
         <v>83</v>
       </c>
       <c r="I62" cm="1">
-        <f t="array" ref="I62">IF(E62="2DSB", IF(H62="R1", 67, 46), IF(E62="1DSB", IF(H62="R1", 67, 46), IF(E62="2DSBanti", IF(H62="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I62">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J62" t="str">
@@ -8396,7 +8396,7 @@
         <v>83</v>
       </c>
       <c r="I63" cm="1">
-        <f t="array" ref="I63">IF(E63="2DSB", IF(H63="R1", 67, 46), IF(E63="1DSB", IF(H63="R1", 67, 46), IF(E63="2DSBanti", IF(H63="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I63">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J63" t="str">
@@ -8450,7 +8450,7 @@
         <v>83</v>
       </c>
       <c r="I64" cm="1">
-        <f t="array" ref="I64">IF(E64="2DSB", IF(H64="R1", 67, 46), IF(E64="1DSB", IF(H64="R1", 67, 46), IF(E64="2DSBanti", IF(H64="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I64">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J64" t="str">
@@ -8504,7 +8504,7 @@
         <v>83</v>
       </c>
       <c r="I65" cm="1">
-        <f t="array" ref="I65">IF(E65="2DSB", IF(H65="R1", 67, 46), IF(E65="1DSB", IF(H65="R1", 67, 46), IF(E65="2DSBanti", IF(H65="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I65">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J65" t="str">
@@ -8558,7 +8558,7 @@
         <v>83</v>
       </c>
       <c r="I66" cm="1">
-        <f t="array" ref="I66">IF(E66="2DSB", IF(H66="R1", 67, 46), IF(E66="1DSB", IF(H66="R1", 67, 46), IF(E66="2DSBanti", IF(H66="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I66">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J66" t="str">
@@ -8612,7 +8612,7 @@
         <v>83</v>
       </c>
       <c r="I67" cm="1">
-        <f t="array" ref="I67">IF(E67="2DSB", IF(H67="R1", 67, 46), IF(E67="1DSB", IF(H67="R1", 67, 46), IF(E67="2DSBanti", IF(H67="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I67">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J67" t="str">
@@ -8666,7 +8666,7 @@
         <v>83</v>
       </c>
       <c r="I68" cm="1">
-        <f t="array" ref="I68">IF(E68="2DSB", IF(H68="R1", 67, 46), IF(E68="1DSB", IF(H68="R1", 67, 46), IF(E68="2DSBanti", IF(H68="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I68">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J68" t="str">
@@ -8720,7 +8720,7 @@
         <v>83</v>
       </c>
       <c r="I69" cm="1">
-        <f t="array" ref="I69">IF(E69="2DSB", IF(H69="R1", 67, 46), IF(E69="1DSB", IF(H69="R1", 67, 46), IF(E69="2DSBanti", IF(H69="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I69">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J69" t="str">
@@ -8774,7 +8774,7 @@
         <v>83</v>
       </c>
       <c r="I70" cm="1">
-        <f t="array" ref="I70">IF(E70="2DSB", IF(H70="R1", 67, 46), IF(E70="1DSB", IF(H70="R1", 67, 46), IF(E70="2DSBanti", IF(H70="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I70">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J70" t="str">
@@ -8828,7 +8828,7 @@
         <v>83</v>
       </c>
       <c r="I71" cm="1">
-        <f t="array" ref="I71">IF(E71="2DSB", IF(H71="R1", 67, 46), IF(E71="1DSB", IF(H71="R1", 67, 46), IF(E71="2DSBanti", IF(H71="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I71">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J71" t="str">
@@ -8882,7 +8882,7 @@
         <v>83</v>
       </c>
       <c r="I72" cm="1">
-        <f t="array" ref="I72">IF(E72="2DSB", IF(H72="R1", 67, 46), IF(E72="1DSB", IF(H72="R1", 67, 46), IF(E72="2DSBanti", IF(H72="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I72">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J72" t="str">
@@ -8936,7 +8936,7 @@
         <v>83</v>
       </c>
       <c r="I73" cm="1">
-        <f t="array" ref="I73">IF(E73="2DSB", IF(H73="R1", 67, 46), IF(E73="1DSB", IF(H73="R1", 67, 46), IF(E73="2DSBanti", IF(H73="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I73">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J73" t="str">
@@ -8990,7 +8990,7 @@
         <v>84</v>
       </c>
       <c r="I74" cm="1">
-        <f t="array" ref="I74">IF(E74="2DSB", IF(H74="R1", 67, 46), IF(E74="1DSB", IF(H74="R1", 67, 46), IF(E74="2DSBanti", IF(H74="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I74">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J74" t="str">
@@ -9044,7 +9044,7 @@
         <v>84</v>
       </c>
       <c r="I75" cm="1">
-        <f t="array" ref="I75">IF(E75="2DSB", IF(H75="R1", 67, 46), IF(E75="1DSB", IF(H75="R1", 67, 46), IF(E75="2DSBanti", IF(H75="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I75">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J75" t="str">
@@ -9098,7 +9098,7 @@
         <v>84</v>
       </c>
       <c r="I76" cm="1">
-        <f t="array" ref="I76">IF(E76="2DSB", IF(H76="R1", 67, 46), IF(E76="1DSB", IF(H76="R1", 67, 46), IF(E76="2DSBanti", IF(H76="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I76">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J76" t="str">
@@ -9152,7 +9152,7 @@
         <v>84</v>
       </c>
       <c r="I77" cm="1">
-        <f t="array" ref="I77">IF(E77="2DSB", IF(H77="R1", 67, 46), IF(E77="1DSB", IF(H77="R1", 67, 46), IF(E77="2DSBanti", IF(H77="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I77">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J77" t="str">
@@ -9206,7 +9206,7 @@
         <v>84</v>
       </c>
       <c r="I78" cm="1">
-        <f t="array" ref="I78">IF(E78="2DSB", IF(H78="R1", 67, 46), IF(E78="1DSB", IF(H78="R1", 67, 46), IF(E78="2DSBanti", IF(H78="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I78">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J78" t="str">
@@ -9260,7 +9260,7 @@
         <v>84</v>
       </c>
       <c r="I79" cm="1">
-        <f t="array" ref="I79">IF(E79="2DSB", IF(H79="R1", 67, 46), IF(E79="1DSB", IF(H79="R1", 67, 46), IF(E79="2DSBanti", IF(H79="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I79">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J79" t="str">
@@ -9314,7 +9314,7 @@
         <v>84</v>
       </c>
       <c r="I80" cm="1">
-        <f t="array" ref="I80">IF(E80="2DSB", IF(H80="R1", 67, 46), IF(E80="1DSB", IF(H80="R1", 67, 46), IF(E80="2DSBanti", IF(H80="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I80">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J80" t="str">
@@ -9368,7 +9368,7 @@
         <v>84</v>
       </c>
       <c r="I81" cm="1">
-        <f t="array" ref="I81">IF(E81="2DSB", IF(H81="R1", 67, 46), IF(E81="1DSB", IF(H81="R1", 67, 46), IF(E81="2DSBanti", IF(H81="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I81">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J81" t="str">
@@ -9422,7 +9422,7 @@
         <v>84</v>
       </c>
       <c r="I82" cm="1">
-        <f t="array" ref="I82">IF(E82="2DSB", IF(H82="R1", 67, 46), IF(E82="1DSB", IF(H82="R1", 67, 46), IF(E82="2DSBanti", IF(H82="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I82">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J82" t="str">
@@ -9476,7 +9476,7 @@
         <v>84</v>
       </c>
       <c r="I83" cm="1">
-        <f t="array" ref="I83">IF(E83="2DSB", IF(H83="R1", 67, 46), IF(E83="1DSB", IF(H83="R1", 67, 46), IF(E83="2DSBanti", IF(H83="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I83">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J83" t="str">
@@ -9530,7 +9530,7 @@
         <v>84</v>
       </c>
       <c r="I84" cm="1">
-        <f t="array" ref="I84">IF(E84="2DSB", IF(H84="R1", 67, 46), IF(E84="1DSB", IF(H84="R1", 67, 46), IF(E84="2DSBanti", IF(H84="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I84">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J84" t="str">
@@ -9584,7 +9584,7 @@
         <v>84</v>
       </c>
       <c r="I85" cm="1">
-        <f t="array" ref="I85">IF(E85="2DSB", IF(H85="R1", 67, 46), IF(E85="1DSB", IF(H85="R1", 67, 46), IF(E85="2DSBanti", IF(H85="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I85">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J85" t="str">
@@ -9638,7 +9638,7 @@
         <v>84</v>
       </c>
       <c r="I86" cm="1">
-        <f t="array" ref="I86">IF(E86="2DSB", IF(H86="R1", 67, 46), IF(E86="1DSB", IF(H86="R1", 67, 46), IF(E86="2DSBanti", IF(H86="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I86">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J86" t="str">
@@ -9692,7 +9692,7 @@
         <v>84</v>
       </c>
       <c r="I87" cm="1">
-        <f t="array" ref="I87">IF(E87="2DSB", IF(H87="R1", 67, 46), IF(E87="1DSB", IF(H87="R1", 67, 46), IF(E87="2DSBanti", IF(H87="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I87">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J87" t="str">
@@ -9746,7 +9746,7 @@
         <v>84</v>
       </c>
       <c r="I88" cm="1">
-        <f t="array" ref="I88">IF(E88="2DSB", IF(H88="R1", 67, 46), IF(E88="1DSB", IF(H88="R1", 67, 46), IF(E88="2DSBanti", IF(H88="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I88">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J88" t="str">
@@ -9800,7 +9800,7 @@
         <v>84</v>
       </c>
       <c r="I89" cm="1">
-        <f t="array" ref="I89">IF(E89="2DSB", IF(H89="R1", 67, 46), IF(E89="1DSB", IF(H89="R1", 67, 46), IF(E89="2DSBanti", IF(H89="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I89">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J89" t="str">
@@ -9854,7 +9854,7 @@
         <v>84</v>
       </c>
       <c r="I90" cm="1">
-        <f t="array" ref="I90">IF(E90="2DSB", IF(H90="R1", 67, 46), IF(E90="1DSB", IF(H90="R1", 67, 46), IF(E90="2DSBanti", IF(H90="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I90">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J90" t="str">
@@ -9908,7 +9908,7 @@
         <v>84</v>
       </c>
       <c r="I91" cm="1">
-        <f t="array" ref="I91">IF(E91="2DSB", IF(H91="R1", 67, 46), IF(E91="1DSB", IF(H91="R1", 67, 46), IF(E91="2DSBanti", IF(H91="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I91">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J91" t="str">
@@ -9962,7 +9962,7 @@
         <v>84</v>
       </c>
       <c r="I92" cm="1">
-        <f t="array" ref="I92">IF(E92="2DSB", IF(H92="R1", 67, 46), IF(E92="1DSB", IF(H92="R1", 67, 46), IF(E92="2DSBanti", IF(H92="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I92">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J92" t="str">
@@ -10016,7 +10016,7 @@
         <v>84</v>
       </c>
       <c r="I93" cm="1">
-        <f t="array" ref="I93">IF(E93="2DSB", IF(H93="R1", 67, 46), IF(E93="1DSB", IF(H93="R1", 67, 46), IF(E93="2DSBanti", IF(H93="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I93">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J93" t="str">
@@ -10070,7 +10070,7 @@
         <v>84</v>
       </c>
       <c r="I94" cm="1">
-        <f t="array" ref="I94">IF(E94="2DSB", IF(H94="R1", 67, 46), IF(E94="1DSB", IF(H94="R1", 67, 46), IF(E94="2DSBanti", IF(H94="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I94">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J94" t="str">
@@ -10124,7 +10124,7 @@
         <v>84</v>
       </c>
       <c r="I95" cm="1">
-        <f t="array" ref="I95">IF(E95="2DSB", IF(H95="R1", 67, 46), IF(E95="1DSB", IF(H95="R1", 67, 46), IF(E95="2DSBanti", IF(H95="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I95">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J95" t="str">
@@ -10178,7 +10178,7 @@
         <v>84</v>
       </c>
       <c r="I96" cm="1">
-        <f t="array" ref="I96">IF(E96="2DSB", IF(H96="R1", 67, 46), IF(E96="1DSB", IF(H96="R1", 67, 46), IF(E96="2DSBanti", IF(H96="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I96">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J96" t="str">
@@ -10232,7 +10232,7 @@
         <v>84</v>
       </c>
       <c r="I97" cm="1">
-        <f t="array" ref="I97">IF(E97="2DSB", IF(H97="R1", 67, 46), IF(E97="1DSB", IF(H97="R1", 67, 46), IF(E97="2DSBanti", IF(H97="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I97">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J97" t="str">
@@ -10286,7 +10286,7 @@
         <v>83</v>
       </c>
       <c r="I98" cm="1">
-        <f t="array" ref="I98">IF(E98="2DSB", IF(H98="R1", 67, 46), IF(E98="1DSB", IF(H98="R1", 67, 46), IF(E98="2DSBanti", IF(H98="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I98">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J98" s="2" t="str">
@@ -10340,7 +10340,7 @@
         <v>83</v>
       </c>
       <c r="I99" cm="1">
-        <f t="array" ref="I99">IF(E99="2DSB", IF(H99="R1", 67, 46), IF(E99="1DSB", IF(H99="R1", 67, 46), IF(E99="2DSBanti", IF(H99="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I99">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J99" s="2" t="str">
@@ -10394,7 +10394,7 @@
         <v>83</v>
       </c>
       <c r="I100" cm="1">
-        <f t="array" ref="I100">IF(E100="2DSB", IF(H100="R1", 67, 46), IF(E100="1DSB", IF(H100="R1", 67, 46), IF(E100="2DSBanti", IF(H100="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I100">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J100" s="2" t="str">
@@ -10448,7 +10448,7 @@
         <v>83</v>
       </c>
       <c r="I101" cm="1">
-        <f t="array" ref="I101">IF(E101="2DSB", IF(H101="R1", 67, 46), IF(E101="1DSB", IF(H101="R1", 67, 46), IF(E101="2DSBanti", IF(H101="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I101">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J101" s="2" t="str">
@@ -10502,7 +10502,7 @@
         <v>83</v>
       </c>
       <c r="I102" cm="1">
-        <f t="array" ref="I102">IF(E102="2DSB", IF(H102="R1", 67, 46), IF(E102="1DSB", IF(H102="R1", 67, 46), IF(E102="2DSBanti", IF(H102="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I102">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J102" s="2" t="str">
@@ -10556,7 +10556,7 @@
         <v>83</v>
       </c>
       <c r="I103" cm="1">
-        <f t="array" ref="I103">IF(E103="2DSB", IF(H103="R1", 67, 46), IF(E103="1DSB", IF(H103="R1", 67, 46), IF(E103="2DSBanti", IF(H103="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I103">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J103" s="2" t="str">
@@ -10610,7 +10610,7 @@
         <v>83</v>
       </c>
       <c r="I104" cm="1">
-        <f t="array" ref="I104">IF(E104="2DSB", IF(H104="R1", 67, 46), IF(E104="1DSB", IF(H104="R1", 67, 46), IF(E104="2DSBanti", IF(H104="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I104">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J104" s="2" t="str">
@@ -10664,7 +10664,7 @@
         <v>83</v>
       </c>
       <c r="I105" cm="1">
-        <f t="array" ref="I105">IF(E105="2DSB", IF(H105="R1", 67, 46), IF(E105="1DSB", IF(H105="R1", 67, 46), IF(E105="2DSBanti", IF(H105="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I105">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J105" s="2" t="str">
@@ -10718,7 +10718,7 @@
         <v>83</v>
       </c>
       <c r="I106" cm="1">
-        <f t="array" ref="I106">IF(E106="2DSB", IF(H106="R1", 67, 46), IF(E106="1DSB", IF(H106="R1", 67, 46), IF(E106="2DSBanti", IF(H106="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I106">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J106" s="2" t="str">
@@ -10772,7 +10772,7 @@
         <v>83</v>
       </c>
       <c r="I107" cm="1">
-        <f t="array" ref="I107">IF(E107="2DSB", IF(H107="R1", 67, 46), IF(E107="1DSB", IF(H107="R1", 67, 46), IF(E107="2DSBanti", IF(H107="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I107">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J107" s="2" t="str">
@@ -10826,7 +10826,7 @@
         <v>83</v>
       </c>
       <c r="I108" cm="1">
-        <f t="array" ref="I108">IF(E108="2DSB", IF(H108="R1", 67, 46), IF(E108="1DSB", IF(H108="R1", 67, 46), IF(E108="2DSBanti", IF(H108="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I108">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J108" s="2" t="str">
@@ -10880,7 +10880,7 @@
         <v>83</v>
       </c>
       <c r="I109" cm="1">
-        <f t="array" ref="I109">IF(E109="2DSB", IF(H109="R1", 67, 46), IF(E109="1DSB", IF(H109="R1", 67, 46), IF(E109="2DSBanti", IF(H109="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I109">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J109" s="2" t="str">
@@ -10934,7 +10934,7 @@
         <v>83</v>
       </c>
       <c r="I110" cm="1">
-        <f t="array" ref="I110">IF(E110="2DSB", IF(H110="R1", 67, 46), IF(E110="1DSB", IF(H110="R1", 67, 46), IF(E110="2DSBanti", IF(H110="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I110">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J110" s="2" t="str">
@@ -10988,7 +10988,7 @@
         <v>83</v>
       </c>
       <c r="I111" cm="1">
-        <f t="array" ref="I111">IF(E111="2DSB", IF(H111="R1", 67, 46), IF(E111="1DSB", IF(H111="R1", 67, 46), IF(E111="2DSBanti", IF(H111="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I111">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J111" s="2" t="str">
@@ -11042,7 +11042,7 @@
         <v>83</v>
       </c>
       <c r="I112" cm="1">
-        <f t="array" ref="I112">IF(E112="2DSB", IF(H112="R1", 67, 46), IF(E112="1DSB", IF(H112="R1", 67, 46), IF(E112="2DSBanti", IF(H112="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I112">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J112" s="2" t="str">
@@ -11096,7 +11096,7 @@
         <v>83</v>
       </c>
       <c r="I113" cm="1">
-        <f t="array" ref="I113">IF(E113="2DSB", IF(H113="R1", 67, 46), IF(E113="1DSB", IF(H113="R1", 67, 46), IF(E113="2DSBanti", IF(H113="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I113">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J113" s="2" t="str">
@@ -11150,7 +11150,7 @@
         <v>83</v>
       </c>
       <c r="I114" cm="1">
-        <f t="array" ref="I114">IF(E114="2DSB", IF(H114="R1", 67, 46), IF(E114="1DSB", IF(H114="R1", 67, 46), IF(E114="2DSBanti", IF(H114="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I114">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J114" s="2" t="str">
@@ -11204,7 +11204,7 @@
         <v>83</v>
       </c>
       <c r="I115" cm="1">
-        <f t="array" ref="I115">IF(E115="2DSB", IF(H115="R1", 67, 46), IF(E115="1DSB", IF(H115="R1", 67, 46), IF(E115="2DSBanti", IF(H115="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I115">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J115" s="2" t="str">
@@ -11258,7 +11258,7 @@
         <v>83</v>
       </c>
       <c r="I116" cm="1">
-        <f t="array" ref="I116">IF(E116="2DSB", IF(H116="R1", 67, 46), IF(E116="1DSB", IF(H116="R1", 67, 46), IF(E116="2DSBanti", IF(H116="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I116">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J116" s="2" t="str">
@@ -11312,7 +11312,7 @@
         <v>83</v>
       </c>
       <c r="I117" cm="1">
-        <f t="array" ref="I117">IF(E117="2DSB", IF(H117="R1", 67, 46), IF(E117="1DSB", IF(H117="R1", 67, 46), IF(E117="2DSBanti", IF(H117="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I117">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J117" s="2" t="str">
@@ -11366,7 +11366,7 @@
         <v>83</v>
       </c>
       <c r="I118" cm="1">
-        <f t="array" ref="I118">IF(E118="2DSB", IF(H118="R1", 67, 46), IF(E118="1DSB", IF(H118="R1", 67, 46), IF(E118="2DSBanti", IF(H118="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I118">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J118" s="2" t="str">
@@ -11420,7 +11420,7 @@
         <v>83</v>
       </c>
       <c r="I119" cm="1">
-        <f t="array" ref="I119">IF(E119="2DSB", IF(H119="R1", 67, 46), IF(E119="1DSB", IF(H119="R1", 67, 46), IF(E119="2DSBanti", IF(H119="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I119">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J119" s="2" t="str">
@@ -11474,7 +11474,7 @@
         <v>83</v>
       </c>
       <c r="I120" cm="1">
-        <f t="array" ref="I120">IF(E120="2DSB", IF(H120="R1", 67, 46), IF(E120="1DSB", IF(H120="R1", 67, 46), IF(E120="2DSBanti", IF(H120="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I120">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J120" s="2" t="str">
@@ -11528,7 +11528,7 @@
         <v>83</v>
       </c>
       <c r="I121" cm="1">
-        <f t="array" ref="I121">IF(E121="2DSB", IF(H121="R1", 67, 46), IF(E121="1DSB", IF(H121="R1", 67, 46), IF(E121="2DSBanti", IF(H121="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I121">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>97</v>
       </c>
       <c r="J121" s="2" t="str">
@@ -11582,7 +11582,7 @@
         <v>84</v>
       </c>
       <c r="I122" cm="1">
-        <f t="array" ref="I122">IF(E122="2DSB", IF(H122="R1", 67, 46), IF(E122="1DSB", IF(H122="R1", 67, 46), IF(E122="2DSBanti", IF(H122="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I122">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J122" s="2" t="str">
@@ -11636,7 +11636,7 @@
         <v>84</v>
       </c>
       <c r="I123" cm="1">
-        <f t="array" ref="I123">IF(E123="2DSB", IF(H123="R1", 67, 46), IF(E123="1DSB", IF(H123="R1", 67, 46), IF(E123="2DSBanti", IF(H123="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I123">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J123" s="2" t="str">
@@ -11690,7 +11690,7 @@
         <v>84</v>
       </c>
       <c r="I124" cm="1">
-        <f t="array" ref="I124">IF(E124="2DSB", IF(H124="R1", 67, 46), IF(E124="1DSB", IF(H124="R1", 67, 46), IF(E124="2DSBanti", IF(H124="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I124">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J124" s="2" t="str">
@@ -11744,7 +11744,7 @@
         <v>84</v>
       </c>
       <c r="I125" cm="1">
-        <f t="array" ref="I125">IF(E125="2DSB", IF(H125="R1", 67, 46), IF(E125="1DSB", IF(H125="R1", 67, 46), IF(E125="2DSBanti", IF(H125="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I125">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J125" s="2" t="str">
@@ -11798,7 +11798,7 @@
         <v>84</v>
       </c>
       <c r="I126" cm="1">
-        <f t="array" ref="I126">IF(E126="2DSB", IF(H126="R1", 67, 46), IF(E126="1DSB", IF(H126="R1", 67, 46), IF(E126="2DSBanti", IF(H126="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I126">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J126" s="2" t="str">
@@ -11852,7 +11852,7 @@
         <v>84</v>
       </c>
       <c r="I127" cm="1">
-        <f t="array" ref="I127">IF(E127="2DSB", IF(H127="R1", 67, 46), IF(E127="1DSB", IF(H127="R1", 67, 46), IF(E127="2DSBanti", IF(H127="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I127">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J127" s="2" t="str">
@@ -11906,7 +11906,7 @@
         <v>84</v>
       </c>
       <c r="I128" cm="1">
-        <f t="array" ref="I128">IF(E128="2DSB", IF(H128="R1", 67, 46), IF(E128="1DSB", IF(H128="R1", 67, 46), IF(E128="2DSBanti", IF(H128="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I128">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J128" s="2" t="str">
@@ -11960,7 +11960,7 @@
         <v>84</v>
       </c>
       <c r="I129" cm="1">
-        <f t="array" ref="I129">IF(E129="2DSB", IF(H129="R1", 67, 46), IF(E129="1DSB", IF(H129="R1", 67, 46), IF(E129="2DSBanti", IF(H129="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I129">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J129" s="2" t="str">
@@ -12014,7 +12014,7 @@
         <v>84</v>
       </c>
       <c r="I130" cm="1">
-        <f t="array" ref="I130">IF(E130="2DSB", IF(H130="R1", 67, 46), IF(E130="1DSB", IF(H130="R1", 67, 46), IF(E130="2DSBanti", IF(H130="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I130">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J130" s="2" t="str">
@@ -12068,7 +12068,7 @@
         <v>84</v>
       </c>
       <c r="I131" cm="1">
-        <f t="array" ref="I131">IF(E131="2DSB", IF(H131="R1", 67, 46), IF(E131="1DSB", IF(H131="R1", 67, 46), IF(E131="2DSBanti", IF(H131="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I131">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J131" s="2" t="str">
@@ -12122,7 +12122,7 @@
         <v>84</v>
       </c>
       <c r="I132" cm="1">
-        <f t="array" ref="I132">IF(E132="2DSB", IF(H132="R1", 67, 46), IF(E132="1DSB", IF(H132="R1", 67, 46), IF(E132="2DSBanti", IF(H132="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I132">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J132" s="2" t="str">
@@ -12176,7 +12176,7 @@
         <v>84</v>
       </c>
       <c r="I133" cm="1">
-        <f t="array" ref="I133">IF(E133="2DSB", IF(H133="R1", 67, 46), IF(E133="1DSB", IF(H133="R1", 67, 46), IF(E133="2DSBanti", IF(H133="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I133">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J133" s="2" t="str">
@@ -12230,7 +12230,7 @@
         <v>84</v>
       </c>
       <c r="I134" cm="1">
-        <f t="array" ref="I134">IF(E134="2DSB", IF(H134="R1", 67, 46), IF(E134="1DSB", IF(H134="R1", 67, 46), IF(E134="2DSBanti", IF(H134="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I134">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J134" s="2" t="str">
@@ -12284,7 +12284,7 @@
         <v>84</v>
       </c>
       <c r="I135" cm="1">
-        <f t="array" ref="I135">IF(E135="2DSB", IF(H135="R1", 67, 46), IF(E135="1DSB", IF(H135="R1", 67, 46), IF(E135="2DSBanti", IF(H135="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I135">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J135" s="2" t="str">
@@ -12338,7 +12338,7 @@
         <v>84</v>
       </c>
       <c r="I136" cm="1">
-        <f t="array" ref="I136">IF(E136="2DSB", IF(H136="R1", 67, 46), IF(E136="1DSB", IF(H136="R1", 67, 46), IF(E136="2DSBanti", IF(H136="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I136">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J136" s="2" t="str">
@@ -12392,7 +12392,7 @@
         <v>84</v>
       </c>
       <c r="I137" cm="1">
-        <f t="array" ref="I137">IF(E137="2DSB", IF(H137="R1", 67, 46), IF(E137="1DSB", IF(H137="R1", 67, 46), IF(E137="2DSBanti", IF(H137="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I137">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J137" s="2" t="str">
@@ -12446,7 +12446,7 @@
         <v>84</v>
       </c>
       <c r="I138" cm="1">
-        <f t="array" ref="I138">IF(E138="2DSB", IF(H138="R1", 67, 46), IF(E138="1DSB", IF(H138="R1", 67, 46), IF(E138="2DSBanti", IF(H138="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I138">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J138" s="2" t="str">
@@ -12500,7 +12500,7 @@
         <v>84</v>
       </c>
       <c r="I139" cm="1">
-        <f t="array" ref="I139">IF(E139="2DSB", IF(H139="R1", 67, 46), IF(E139="1DSB", IF(H139="R1", 67, 46), IF(E139="2DSBanti", IF(H139="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I139">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J139" s="2" t="str">
@@ -12554,7 +12554,7 @@
         <v>84</v>
       </c>
       <c r="I140" cm="1">
-        <f t="array" ref="I140">IF(E140="2DSB", IF(H140="R1", 67, 46), IF(E140="1DSB", IF(H140="R1", 67, 46), IF(E140="2DSBanti", IF(H140="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I140">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J140" s="2" t="str">
@@ -12608,7 +12608,7 @@
         <v>84</v>
       </c>
       <c r="I141" cm="1">
-        <f t="array" ref="I141">IF(E141="2DSB", IF(H141="R1", 67, 46), IF(E141="1DSB", IF(H141="R1", 67, 46), IF(E141="2DSBanti", IF(H141="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I141">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J141" s="2" t="str">
@@ -12662,7 +12662,7 @@
         <v>84</v>
       </c>
       <c r="I142" cm="1">
-        <f t="array" ref="I142">IF(E142="2DSB", IF(H142="R1", 67, 46), IF(E142="1DSB", IF(H142="R1", 67, 46), IF(E142="2DSBanti", IF(H142="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I142">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J142" s="2" t="str">
@@ -12716,7 +12716,7 @@
         <v>84</v>
       </c>
       <c r="I143" cm="1">
-        <f t="array" ref="I143">IF(E143="2DSB", IF(H143="R1", 67, 46), IF(E143="1DSB", IF(H143="R1", 67, 46), IF(E143="2DSBanti", IF(H143="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I143">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J143" s="2" t="str">
@@ -12770,7 +12770,7 @@
         <v>84</v>
       </c>
       <c r="I144" cm="1">
-        <f t="array" ref="I144">IF(E144="2DSB", IF(H144="R1", 67, 46), IF(E144="1DSB", IF(H144="R1", 67, 46), IF(E144="2DSBanti", IF(H144="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I144">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J144" s="2" t="str">
@@ -12824,7 +12824,7 @@
         <v>84</v>
       </c>
       <c r="I145" cm="1">
-        <f t="array" ref="I145">IF(E145="2DSB", IF(H145="R1", 67, 46), IF(E145="1DSB", IF(H145="R1", 67, 46), IF(E145="2DSBanti", IF(H145="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I145">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>76</v>
       </c>
       <c r="J145" s="2" t="str">
@@ -12878,8 +12878,8 @@
         <v>83</v>
       </c>
       <c r="I146" cm="1">
-        <f t="array" ref="I146">IF(E146="2DSB", IF(H146="R1", 67, 46), IF(E146="1DSB", IF(H146="R1", 67, 46), IF(E146="2DSBanti", IF(H146="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I146">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J146" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -12903,7 +12903,7 @@
       </c>
       <c r="O146" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl349_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl349_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl349_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl349_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
@@ -12932,8 +12932,8 @@
         <v>83</v>
       </c>
       <c r="I147" cm="1">
-        <f t="array" ref="I147">IF(E147="2DSB", IF(H147="R1", 67, 46), IF(E147="1DSB", IF(H147="R1", 67, 46), IF(E147="2DSBanti", IF(H147="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I147">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J147" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -12957,7 +12957,7 @@
       </c>
       <c r="O147" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl350_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl350_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl350_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl350_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
@@ -12986,8 +12986,8 @@
         <v>83</v>
       </c>
       <c r="I148" cm="1">
-        <f t="array" ref="I148">IF(E148="2DSB", IF(H148="R1", 67, 46), IF(E148="1DSB", IF(H148="R1", 67, 46), IF(E148="2DSBanti", IF(H148="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I148">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J148" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -13011,7 +13011,7 @@
       </c>
       <c r="O148" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl351_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl351_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl351_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl351_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.25">
@@ -13040,8 +13040,8 @@
         <v>83</v>
       </c>
       <c r="I149" cm="1">
-        <f t="array" ref="I149">IF(E149="2DSB", IF(H149="R1", 67, 46), IF(E149="1DSB", IF(H149="R1", 67, 46), IF(E149="2DSBanti", IF(H149="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I149">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J149" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -13065,7 +13065,7 @@
       </c>
       <c r="O149" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl352_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl352_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl352_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl352_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
@@ -13094,8 +13094,8 @@
         <v>83</v>
       </c>
       <c r="I150" cm="1">
-        <f t="array" ref="I150">IF(E150="2DSB", IF(H150="R1", 67, 46), IF(E150="1DSB", IF(H150="R1", 67, 46), IF(E150="2DSBanti", IF(H150="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I150">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J150" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -13119,7 +13119,7 @@
       </c>
       <c r="O150" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl353_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl353_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl353_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl353_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
@@ -13148,8 +13148,8 @@
         <v>83</v>
       </c>
       <c r="I151" cm="1">
-        <f t="array" ref="I151">IF(E151="2DSB", IF(H151="R1", 67, 46), IF(E151="1DSB", IF(H151="R1", 67, 46), IF(E151="2DSBanti", IF(H151="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I151">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J151" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -13173,7 +13173,7 @@
       </c>
       <c r="O151" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl354_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl354_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl354_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl354_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.25">
@@ -13202,8 +13202,8 @@
         <v>83</v>
       </c>
       <c r="I152" cm="1">
-        <f t="array" ref="I152">IF(E152="2DSB", IF(H152="R1", 67, 46), IF(E152="1DSB", IF(H152="R1", 67, 46), IF(E152="2DSBanti", IF(H152="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I152">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J152" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -13227,7 +13227,7 @@
       </c>
       <c r="O152" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl355_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl355_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl355_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl355_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.25">
@@ -13256,8 +13256,8 @@
         <v>83</v>
       </c>
       <c r="I153" cm="1">
-        <f t="array" ref="I153">IF(E153="2DSB", IF(H153="R1", 67, 46), IF(E153="1DSB", IF(H153="R1", 67, 46), IF(E153="2DSBanti", IF(H153="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
-        <v>50</v>
+        <f t="array" ref="I153">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <v>66</v>
       </c>
       <c r="J153" t="str">
         <f>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</f>
@@ -13281,7 +13281,7 @@
       </c>
       <c r="O153" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl356_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl356_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl356_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl356_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet</v>
       </c>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.25">
@@ -13310,7 +13310,7 @@
         <v>84</v>
       </c>
       <c r="I154" cm="1">
-        <f t="array" ref="I154">IF(E154="2DSB", IF(H154="R1", 67, 46), IF(E154="1DSB", IF(H154="R1", 67, 46), IF(E154="2DSBanti", IF(H154="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I154">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J154" t="str">
@@ -13364,7 +13364,7 @@
         <v>84</v>
       </c>
       <c r="I155" cm="1">
-        <f t="array" ref="I155">IF(E155="2DSB", IF(H155="R1", 67, 46), IF(E155="1DSB", IF(H155="R1", 67, 46), IF(E155="2DSBanti", IF(H155="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I155">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J155" t="str">
@@ -13418,7 +13418,7 @@
         <v>84</v>
       </c>
       <c r="I156" cm="1">
-        <f t="array" ref="I156">IF(E156="2DSB", IF(H156="R1", 67, 46), IF(E156="1DSB", IF(H156="R1", 67, 46), IF(E156="2DSBanti", IF(H156="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I156">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J156" t="str">
@@ -13472,7 +13472,7 @@
         <v>84</v>
       </c>
       <c r="I157" cm="1">
-        <f t="array" ref="I157">IF(E157="2DSB", IF(H157="R1", 67, 46), IF(E157="1DSB", IF(H157="R1", 67, 46), IF(E157="2DSBanti", IF(H157="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I157">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J157" t="str">
@@ -13526,7 +13526,7 @@
         <v>84</v>
       </c>
       <c r="I158" cm="1">
-        <f t="array" ref="I158">IF(E158="2DSB", IF(H158="R1", 67, 46), IF(E158="1DSB", IF(H158="R1", 67, 46), IF(E158="2DSBanti", IF(H158="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I158">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J158" t="str">
@@ -13580,7 +13580,7 @@
         <v>84</v>
       </c>
       <c r="I159" cm="1">
-        <f t="array" ref="I159">IF(E159="2DSB", IF(H159="R1", 67, 46), IF(E159="1DSB", IF(H159="R1", 67, 46), IF(E159="2DSBanti", IF(H159="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I159">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J159" t="str">
@@ -13634,7 +13634,7 @@
         <v>84</v>
       </c>
       <c r="I160" cm="1">
-        <f t="array" ref="I160">IF(E160="2DSB", IF(H160="R1", 67, 46), IF(E160="1DSB", IF(H160="R1", 67, 46), IF(E160="2DSBanti", IF(H160="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I160">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J160" t="str">
@@ -13688,7 +13688,7 @@
         <v>84</v>
       </c>
       <c r="I161" cm="1">
-        <f t="array" ref="I161">IF(E161="2DSB", IF(H161="R1", 67, 46), IF(E161="1DSB", IF(H161="R1", 67, 46), IF(E161="2DSBanti", IF(H161="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I161">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>47</v>
       </c>
       <c r="J161" t="str">
@@ -13742,7 +13742,7 @@
         <v>83</v>
       </c>
       <c r="I162" cm="1">
-        <f t="array" ref="I162">IF(E162="2DSB", IF(H162="R1", 67, 46), IF(E162="1DSB", IF(H162="R1", 67, 46), IF(E162="2DSBanti", IF(H162="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I162">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J162" t="str">
@@ -13796,7 +13796,7 @@
         <v>83</v>
       </c>
       <c r="I163" cm="1">
-        <f t="array" ref="I163">IF(E163="2DSB", IF(H163="R1", 67, 46), IF(E163="1DSB", IF(H163="R1", 67, 46), IF(E163="2DSBanti", IF(H163="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I163">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J163" t="str">
@@ -13850,7 +13850,7 @@
         <v>83</v>
       </c>
       <c r="I164" cm="1">
-        <f t="array" ref="I164">IF(E164="2DSB", IF(H164="R1", 67, 46), IF(E164="1DSB", IF(H164="R1", 67, 46), IF(E164="2DSBanti", IF(H164="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I164">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J164" t="str">
@@ -13904,7 +13904,7 @@
         <v>83</v>
       </c>
       <c r="I165" cm="1">
-        <f t="array" ref="I165">IF(E165="2DSB", IF(H165="R1", 67, 46), IF(E165="1DSB", IF(H165="R1", 67, 46), IF(E165="2DSBanti", IF(H165="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I165">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J165" t="str">
@@ -13958,7 +13958,7 @@
         <v>83</v>
       </c>
       <c r="I166" cm="1">
-        <f t="array" ref="I166">IF(E166="2DSB", IF(H166="R1", 67, 46), IF(E166="1DSB", IF(H166="R1", 67, 46), IF(E166="2DSBanti", IF(H166="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I166">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J166" t="str">
@@ -14012,7 +14012,7 @@
         <v>83</v>
       </c>
       <c r="I167" cm="1">
-        <f t="array" ref="I167">IF(E167="2DSB", IF(H167="R1", 67, 46), IF(E167="1DSB", IF(H167="R1", 67, 46), IF(E167="2DSBanti", IF(H167="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I167">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>67</v>
       </c>
       <c r="J167" t="str">
@@ -14066,7 +14066,7 @@
         <v>84</v>
       </c>
       <c r="I168" cm="1">
-        <f t="array" ref="I168">IF(E168="2DSB", IF(H168="R1", 67, 46), IF(E168="1DSB", IF(H168="R1", 67, 46), IF(E168="2DSBanti", IF(H168="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I168">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J168" t="str">
@@ -14120,7 +14120,7 @@
         <v>84</v>
       </c>
       <c r="I169" cm="1">
-        <f t="array" ref="I169">IF(E169="2DSB", IF(H169="R1", 67, 46), IF(E169="1DSB", IF(H169="R1", 67, 46), IF(E169="2DSBanti", IF(H169="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I169">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J169" t="str">
@@ -14174,7 +14174,7 @@
         <v>84</v>
       </c>
       <c r="I170" cm="1">
-        <f t="array" ref="I170">IF(E170="2DSB", IF(H170="R1", 67, 46), IF(E170="1DSB", IF(H170="R1", 67, 46), IF(E170="2DSBanti", IF(H170="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I170">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J170" t="str">
@@ -14228,7 +14228,7 @@
         <v>84</v>
       </c>
       <c r="I171" cm="1">
-        <f t="array" ref="I171">IF(E171="2DSB", IF(H171="R1", 67, 46), IF(E171="1DSB", IF(H171="R1", 67, 46), IF(E171="2DSBanti", IF(H171="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I171">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J171" t="str">
@@ -14282,7 +14282,7 @@
         <v>84</v>
       </c>
       <c r="I172" cm="1">
-        <f t="array" ref="I172">IF(E172="2DSB", IF(H172="R1", 67, 46), IF(E172="1DSB", IF(H172="R1", 67, 46), IF(E172="2DSBanti", IF(H172="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I172">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J172" t="str">
@@ -14336,7 +14336,7 @@
         <v>84</v>
       </c>
       <c r="I173" cm="1">
-        <f t="array" ref="I173">IF(E173="2DSB", IF(H173="R1", 67, 46), IF(E173="1DSB", IF(H173="R1", 67, 46), IF(E173="2DSBanti", IF(H173="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
+        <f t="array" ref="I173">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</f>
         <v>46</v>
       </c>
       <c r="J173" t="str">
@@ -14516,14 +14516,14 @@
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl313_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl313_KO_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl314_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl314_KO_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl315_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl315_KO_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl349_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl349_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl350_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl350_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl351_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl351_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl352_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl352_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl353_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl353_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl354_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl354_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl355_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl355_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl356_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl356_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl349_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl349_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl350_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl350_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl351_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl351_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl352_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl352_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 66 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl353_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl353_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl354_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl354_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl355_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl355_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl356_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl356_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 66 --quiet
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl349_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_antisense.fa -o libraries_2/yjl349_WT_sgCD_R2_antisense.tsv --min_length 50 -dsb 47 --quiet
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl350_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_antisense.fa -o libraries_2/yjl350_WT_sgCD_R2_antisense.tsv --min_length 50 -dsb 47 --quiet
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl351_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_antisense.fa -o libraries_2/yjl351_WT_sgCD_R2_antisense.tsv --min_length 50 -dsb 47 --quiet
@@ -14560,8 +14560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D704B5-D01A-4D17-9252-416EA08BC871}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:A59"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17429,7 +17429,7 @@
       </c>
       <c r="E38">
         <f ca="1">OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F38" t="str">
         <f ca="1">OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</f>
@@ -17506,7 +17506,7 @@
       </c>
       <c r="E39">
         <f ca="1">OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F39" t="str">
         <f ca="1">OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</f>
@@ -18481,8 +18481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB6E33-93C4-4971-BF44-23A0F65AADA0}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20614,7 +20614,7 @@
       </c>
       <c r="E38">
         <f ca="1">OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F38" t="str">
         <f ca="1">OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20646,7 +20646,7 @@
       </c>
       <c r="M38" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_antisense.tsv -o libraries_4/WT_sgCD_R1_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 50 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment antisense --subst_type without --control none</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_antisense.tsv -o libraries_4/WT_sgCD_R1_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 66 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment antisense --subst_type without --control none</v>
       </c>
       <c r="N38" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</f>
@@ -20671,7 +20671,7 @@
       </c>
       <c r="E39">
         <f ca="1">OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F39" t="str">
         <f ca="1">OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20703,7 +20703,7 @@
       </c>
       <c r="M39" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 50 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without --control none</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 66 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without --control none</v>
       </c>
       <c r="N39" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</f>
@@ -21596,8 +21596,8 @@
 python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense_30bpDown.tsv -o libraries_4/KO_sgB_R2_sense_30bpDown -ref ref_seq/1DSB_R2_sense.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control 30bpDown
 python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch_30bpDown.tsv -o libraries_4/KO_sgB_R2_branch_30bpDown -ref ref_seq/1DSB_R2_branch.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control 30bpDown
 python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv_30bpDown.tsv -o libraries_4/KO_sgB_R2_cmv_30bpDown -ref ref_seq/1DSB_R2_cmv.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control 30bpDown
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_antisense.tsv -o libraries_4/WT_sgCD_R1_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 50 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment antisense --subst_type without --control none
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 50 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_antisense.tsv -o libraries_4/WT_sgCD_R1_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 66 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment antisense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 66 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without --control none
 python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R2_antisense.tsv -o libraries_4/WT_sgCD_R2_antisense -ref ref_seq/2DSBanti_R2_antisense.fa -dsb 47 --dsb_type 2a --strand R2 --hguide CD --cell WT --treatment antisense --subst_type without --control none
 python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R2_splicing.tsv -o libraries_4/WT_sgCD_R2_splicing -ref ref_seq/2DSBanti_R2_splicing.fa -dsb 47 --dsb_type 2a --strand R2 --hguide CD --cell WT --treatment splicing --subst_type without --control none
 python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense_nodsb.tsv -o libraries_4/WT_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control noDSB
@@ -25363,7 +25363,7 @@
       </c>
       <c r="E38">
         <f ca="1">table_3_1[[#This Row],[dsb_pos]]</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F38" t="str">
         <f ca="1">table_3_1[[#This Row],[dsb_type]]</f>
@@ -25424,7 +25424,7 @@
       </c>
       <c r="E39">
         <f ca="1">table_3_1[[#This Row],[dsb_pos]]</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F39" t="str">
         <f ca="1">table_3_1[[#This Row],[dsb_type]]</f>
@@ -26822,7 +26822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
@@ -27035,7 +27035,7 @@
         <v>13</v>
       </c>
       <c r="Q3">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R3">
@@ -27062,7 +27062,7 @@
         <v>7</v>
       </c>
       <c r="X3">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y3" t="str">
@@ -27155,7 +27155,7 @@
         <v>13</v>
       </c>
       <c r="Q4">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R4">
@@ -27182,7 +27182,7 @@
         <v>7</v>
       </c>
       <c r="X4">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y4" t="str">
@@ -27275,7 +27275,7 @@
         <v>13</v>
       </c>
       <c r="Q5">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R5">
@@ -27302,7 +27302,7 @@
         <v>7</v>
       </c>
       <c r="X5">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y5" t="str">
@@ -27395,7 +27395,7 @@
         <v>13</v>
       </c>
       <c r="Q6">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R6">
@@ -27422,7 +27422,7 @@
         <v>7</v>
       </c>
       <c r="X6">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y6" t="str">
@@ -27515,7 +27515,7 @@
         <v>13</v>
       </c>
       <c r="Q7">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R7">
@@ -27542,7 +27542,7 @@
         <v>7</v>
       </c>
       <c r="X7">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y7" t="str">
@@ -27635,7 +27635,7 @@
         <v>13</v>
       </c>
       <c r="Q8">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R8">
@@ -27662,7 +27662,7 @@
         <v>7</v>
       </c>
       <c r="X8">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y8" t="str">
@@ -27755,7 +27755,7 @@
         <v>13</v>
       </c>
       <c r="Q9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R9">
@@ -27782,7 +27782,7 @@
         <v>7</v>
       </c>
       <c r="X9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y9" t="str">
@@ -27875,7 +27875,7 @@
         <v>13</v>
       </c>
       <c r="Q10">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R10">
@@ -27902,7 +27902,7 @@
         <v>7</v>
       </c>
       <c r="X10">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y10" t="str">
@@ -27995,7 +27995,7 @@
         <v>13</v>
       </c>
       <c r="Q11">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R11">
@@ -28022,7 +28022,7 @@
         <v>7</v>
       </c>
       <c r="X11">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y11" t="str">
@@ -28115,7 +28115,7 @@
         <v>13</v>
       </c>
       <c r="Q12">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R12">
@@ -28142,7 +28142,7 @@
         <v>7</v>
       </c>
       <c r="X12">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y12" t="str">
@@ -28235,7 +28235,7 @@
         <v>13</v>
       </c>
       <c r="Q13">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R13">
@@ -28262,7 +28262,7 @@
         <v>7</v>
       </c>
       <c r="X13">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y13" t="str">
@@ -28355,7 +28355,7 @@
         <v>13</v>
       </c>
       <c r="Q14">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R14">
@@ -28382,7 +28382,7 @@
         <v>7</v>
       </c>
       <c r="X14">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>17</v>
       </c>
       <c r="Y14" t="str">
@@ -28475,7 +28475,7 @@
         <v>13</v>
       </c>
       <c r="Q15">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R15">
@@ -28502,7 +28502,7 @@
         <v>6</v>
       </c>
       <c r="X15">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y15" t="str">
@@ -28595,7 +28595,7 @@
         <v>13</v>
       </c>
       <c r="Q16">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R16">
@@ -28622,7 +28622,7 @@
         <v>6</v>
       </c>
       <c r="X16">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y16" t="str">
@@ -28715,7 +28715,7 @@
         <v>13</v>
       </c>
       <c r="Q17">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R17">
@@ -28742,7 +28742,7 @@
         <v>6</v>
       </c>
       <c r="X17">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y17" t="str">
@@ -28835,7 +28835,7 @@
         <v>13</v>
       </c>
       <c r="Q18">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R18">
@@ -28862,7 +28862,7 @@
         <v>6</v>
       </c>
       <c r="X18">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y18" t="str">
@@ -28955,7 +28955,7 @@
         <v>13</v>
       </c>
       <c r="Q19">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R19">
@@ -28982,7 +28982,7 @@
         <v>6</v>
       </c>
       <c r="X19">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y19" t="str">
@@ -29075,7 +29075,7 @@
         <v>13</v>
       </c>
       <c r="Q20">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R20">
@@ -29102,7 +29102,7 @@
         <v>6</v>
       </c>
       <c r="X20">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y20" t="str">
@@ -29195,7 +29195,7 @@
         <v>13</v>
       </c>
       <c r="Q21">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R21">
@@ -29222,7 +29222,7 @@
         <v>5</v>
       </c>
       <c r="X21">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y21" t="str">
@@ -29315,7 +29315,7 @@
         <v>13</v>
       </c>
       <c r="Q22">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R22">
@@ -29342,7 +29342,7 @@
         <v>5</v>
       </c>
       <c r="X22">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y22" t="str">
@@ -29435,7 +29435,7 @@
         <v>13</v>
       </c>
       <c r="Q23">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R23">
@@ -29462,7 +29462,7 @@
         <v>5</v>
       </c>
       <c r="X23">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y23" t="str">
@@ -29555,7 +29555,7 @@
         <v>13</v>
       </c>
       <c r="Q24">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R24">
@@ -29582,7 +29582,7 @@
         <v>5</v>
       </c>
       <c r="X24">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y24" t="str">
@@ -29675,7 +29675,7 @@
         <v>13</v>
       </c>
       <c r="Q25">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R25">
@@ -29702,7 +29702,7 @@
         <v>5</v>
       </c>
       <c r="X25">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y25" t="str">
@@ -29795,7 +29795,7 @@
         <v>13</v>
       </c>
       <c r="Q26">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R26">
@@ -29822,7 +29822,7 @@
         <v>5</v>
       </c>
       <c r="X26">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y26" t="str">
@@ -29915,7 +29915,7 @@
         <v>13</v>
       </c>
       <c r="Q27" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R27" s="9">
@@ -29942,7 +29942,7 @@
         <v>6</v>
       </c>
       <c r="X27" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y27" s="9" t="str">
@@ -30035,7 +30035,7 @@
         <v>13</v>
       </c>
       <c r="Q28" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R28" s="9">
@@ -30062,7 +30062,7 @@
         <v>6</v>
       </c>
       <c r="X28" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y28" s="9" t="str">
@@ -30155,7 +30155,7 @@
         <v>13</v>
       </c>
       <c r="Q29" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R29" s="9">
@@ -30182,7 +30182,7 @@
         <v>6</v>
       </c>
       <c r="X29" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y29" s="9" t="str">
@@ -30275,7 +30275,7 @@
         <v>13</v>
       </c>
       <c r="Q30" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R30" s="9">
@@ -30302,7 +30302,7 @@
         <v>6</v>
       </c>
       <c r="X30" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y30" s="9" t="str">
@@ -30395,7 +30395,7 @@
         <v>13</v>
       </c>
       <c r="Q31" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R31" s="9">
@@ -30422,7 +30422,7 @@
         <v>6</v>
       </c>
       <c r="X31" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y31" s="9" t="str">
@@ -30515,7 +30515,7 @@
         <v>13</v>
       </c>
       <c r="Q32" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-23</v>
       </c>
       <c r="R32" s="9">
@@ -30542,7 +30542,7 @@
         <v>6</v>
       </c>
       <c r="X32" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>19</v>
       </c>
       <c r="Y32" s="9" t="str">
@@ -30635,7 +30635,7 @@
         <v>13</v>
       </c>
       <c r="Q33" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R33" s="9">
@@ -30662,7 +30662,7 @@
         <v>5</v>
       </c>
       <c r="X33" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y33" s="9" t="str">
@@ -30755,7 +30755,7 @@
         <v>13</v>
       </c>
       <c r="Q34" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R34" s="9">
@@ -30782,7 +30782,7 @@
         <v>5</v>
       </c>
       <c r="X34" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y34" s="9" t="str">
@@ -30875,7 +30875,7 @@
         <v>13</v>
       </c>
       <c r="Q35" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R35" s="9">
@@ -30902,7 +30902,7 @@
         <v>5</v>
       </c>
       <c r="X35" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y35" s="9" t="str">
@@ -30995,7 +30995,7 @@
         <v>13</v>
       </c>
       <c r="Q36" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R36" s="9">
@@ -31022,7 +31022,7 @@
         <v>5</v>
       </c>
       <c r="X36" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y36" s="9" t="str">
@@ -31115,7 +31115,7 @@
         <v>13</v>
       </c>
       <c r="Q37" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R37" s="9">
@@ -31142,7 +31142,7 @@
         <v>5</v>
       </c>
       <c r="X37" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y37" s="9" t="str">
@@ -31235,7 +31235,7 @@
         <v>13</v>
       </c>
       <c r="Q38" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
         <v>-22</v>
       </c>
       <c r="R38" s="9">
@@ -31262,7 +31262,7 @@
         <v>5</v>
       </c>
       <c r="X38" s="9">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
         <v>18</v>
       </c>
       <c r="Y38" s="9" t="str">
@@ -31299,7 +31299,7 @@
       </c>
       <c r="E39">
         <f ca="1">OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F39" t="str">
         <f ca="1">OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -31355,8 +31355,8 @@
         <v>13</v>
       </c>
       <c r="Q39">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
-        <v>-18</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <v>-22</v>
       </c>
       <c r="R39">
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 22, IF(table_7_1[[#This Row],[hguide]]="CD", 27, IF(table_7_1[[#This Row],[hguide]]="A", 20, IF(table_7_1[[#This Row],[hguide]]="B", 16, NA())))), NA())</f>
@@ -31364,30 +31364,30 @@
       </c>
       <c r="S39" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT("--range_x ", table_7_1[[#This Row],[range_x0]], " ", table_7_1[[#This Row],[range_x1]], " --range_y ", table_7_1[[#This Row],[range_y0]], " ", table_7_1[[#This Row],[range_y1]]), "")</f>
-        <v>--range_x -12 13 --range_y -18 27</v>
+        <v>--range_x -12 13 --range_y -22 27</v>
       </c>
       <c r="T39" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_x_pos ", table_7_1[[#This Row],[range_x1]] - 1, " --universal_layout_y_axis_y_range ", table_7_1[[#This Row],[range_y0]] + 2.5, " ", table_7_1[[#This Row],[range_y1]] - 1.5, " "), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5 </v>
+        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5 </v>
       </c>
       <c r="U39" t="b">
         <v>1</v>
       </c>
       <c r="V39" t="str">
         <f ca="1">IF(table_7_1[[#This Row],[show_universal_layout_x_axes]], _xlfn.CONCAT(" --universal_layout_x_axis_deletion_y_pos ", table_7_1[[#This Row],[range_y0]] + 1.5, " --universal_layout_x_axis_insertion_y_pos ", table_7_1[[#This Row],[range_y1]] - 0.5, " --universal_layout_x_axis_x_range ", table_7_1[[#This Row],[range_x0]] + 0.5, " ", table_7_1[[#This Row],[range_x1]] - 1.5), "")</f>
-        <v xml:space="preserve"> --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5</v>
+        <v xml:space="preserve"> --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5</v>
       </c>
       <c r="W39">
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 7, IF(table_7_1[[#This Row],[hguide]]="CD", 8, IF(table_7_1[[#This Row],[hguide]]="A", 6, IF(table_7_1[[#This Row],[hguide]]="B", 5, NA())))), NA())</f>
         <v>8</v>
       </c>
       <c r="X39">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
-        <v>14</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <v>17</v>
       </c>
       <c r="Y39" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z39" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
@@ -31398,7 +31398,7 @@
       </c>
       <c r="AB39" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5   --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -31419,7 +31419,7 @@
       </c>
       <c r="E40">
         <f ca="1">OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F40" t="str">
         <f ca="1">OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -31475,8 +31475,8 @@
         <v>13</v>
       </c>
       <c r="Q40">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
-        <v>-18</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <v>-22</v>
       </c>
       <c r="R40">
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 22, IF(table_7_1[[#This Row],[hguide]]="CD", 27, IF(table_7_1[[#This Row],[hguide]]="A", 20, IF(table_7_1[[#This Row],[hguide]]="B", 16, NA())))), NA())</f>
@@ -31484,11 +31484,11 @@
       </c>
       <c r="S40" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT("--range_x ", table_7_1[[#This Row],[range_x0]], " ", table_7_1[[#This Row],[range_x1]], " --range_y ", table_7_1[[#This Row],[range_y0]], " ", table_7_1[[#This Row],[range_y1]]), "")</f>
-        <v>--range_x -12 13 --range_y -18 27</v>
+        <v>--range_x -12 13 --range_y -22 27</v>
       </c>
       <c r="T40" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_x_pos ", table_7_1[[#This Row],[range_x1]] - 1, " --universal_layout_y_axis_y_range ", table_7_1[[#This Row],[range_y0]] + 2.5, " ", table_7_1[[#This Row],[range_y1]] - 1.5, " "), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5 </v>
+        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5 </v>
       </c>
       <c r="U40" t="b">
         <v>0</v>
@@ -31502,12 +31502,12 @@
         <v>8</v>
       </c>
       <c r="X40">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
-        <v>14</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <v>17</v>
       </c>
       <c r="Y40" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z40" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
@@ -31518,7 +31518,7 @@
       </c>
       <c r="AB40" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
@@ -31595,8 +31595,8 @@
         <v>13</v>
       </c>
       <c r="Q41">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
-        <v>-18</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <v>-22</v>
       </c>
       <c r="R41">
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 22, IF(table_7_1[[#This Row],[hguide]]="CD", 27, IF(table_7_1[[#This Row],[hguide]]="A", 20, IF(table_7_1[[#This Row],[hguide]]="B", 16, NA())))), NA())</f>
@@ -31604,11 +31604,11 @@
       </c>
       <c r="S41" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT("--range_x ", table_7_1[[#This Row],[range_x0]], " ", table_7_1[[#This Row],[range_x1]], " --range_y ", table_7_1[[#This Row],[range_y0]], " ", table_7_1[[#This Row],[range_y1]]), "")</f>
-        <v>--range_x -12 13 --range_y -18 27</v>
+        <v>--range_x -12 13 --range_y -22 27</v>
       </c>
       <c r="T41" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_x_pos ", table_7_1[[#This Row],[range_x1]] - 1, " --universal_layout_y_axis_y_range ", table_7_1[[#This Row],[range_y0]] + 2.5, " ", table_7_1[[#This Row],[range_y1]] - 1.5, " "), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5 </v>
+        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5 </v>
       </c>
       <c r="U41" t="b">
         <v>0</v>
@@ -31622,12 +31622,12 @@
         <v>8</v>
       </c>
       <c r="X41">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
-        <v>14</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <v>17</v>
       </c>
       <c r="Y41" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z41" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
@@ -31638,7 +31638,7 @@
       </c>
       <c r="AB41" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
@@ -31715,8 +31715,8 @@
         <v>13</v>
       </c>
       <c r="Q42">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
-        <v>-18</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</f>
+        <v>-22</v>
       </c>
       <c r="R42">
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 22, IF(table_7_1[[#This Row],[hguide]]="CD", 27, IF(table_7_1[[#This Row],[hguide]]="A", 20, IF(table_7_1[[#This Row],[hguide]]="B", 16, NA())))), NA())</f>
@@ -31724,11 +31724,11 @@
       </c>
       <c r="S42" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT("--range_x ", table_7_1[[#This Row],[range_x0]], " ", table_7_1[[#This Row],[range_x1]], " --range_y ", table_7_1[[#This Row],[range_y0]], " ", table_7_1[[#This Row],[range_y1]]), "")</f>
-        <v>--range_x -12 13 --range_y -18 27</v>
+        <v>--range_x -12 13 --range_y -22 27</v>
       </c>
       <c r="T42" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_x_pos ", table_7_1[[#This Row],[range_x1]] - 1, " --universal_layout_y_axis_y_range ", table_7_1[[#This Row],[range_y0]] + 2.5, " ", table_7_1[[#This Row],[range_y1]] - 1.5, " "), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5 </v>
+        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5 </v>
       </c>
       <c r="U42" t="b">
         <v>0</v>
@@ -31742,12 +31742,12 @@
         <v>8</v>
       </c>
       <c r="X42">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
-        <v>14</v>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</f>
+        <v>17</v>
       </c>
       <c r="Y42" t="str">
         <f ca="1">IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z42" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
@@ -31758,7 +31758,7 @@
       </c>
       <c r="AB42" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
@@ -32829,11 +32829,11 @@
       </c>
       <c r="H63" s="2" t="str">
         <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>--range_x -12 13 --range_y -18 27</v>
+        <v>--range_x -12 13 --range_y -22 27</v>
       </c>
       <c r="I63" s="2" t="str">
         <f ca="1">OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5 </v>
+        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5 </v>
       </c>
       <c r="J63" s="2" t="b">
         <v>0</v>
@@ -32844,7 +32844,7 @@
       </c>
       <c r="L63" s="2" t="str">
         <f ca="1">OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="M63" s="2" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</f>
@@ -32855,7 +32855,7 @@
       </c>
       <c r="O63" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -32888,11 +32888,11 @@
       </c>
       <c r="H64" s="2" t="str">
         <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>--range_x -12 13 --range_y -18 27</v>
+        <v>--range_x -12 13 --range_y -22 27</v>
       </c>
       <c r="I64" s="2" t="str">
         <f ca="1">OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5 </v>
+        <v xml:space="preserve"> --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5 </v>
       </c>
       <c r="J64" s="2" t="b">
         <v>0</v>
@@ -32903,7 +32903,7 @@
       </c>
       <c r="L64" s="2" t="str">
         <f ca="1">OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="M64" s="2" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</f>
@@ -32914,7 +32914,7 @@
       </c>
       <c r="O64" s="2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
@@ -32949,10 +32949,10 @@
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5   --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
@@ -32969,8 +32969,8 @@
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 25.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix name of splicing construct.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo_new_antisense.xlsx
+++ b/analyze_nhej/libinfo_new_antisense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E45DB47-3CD2-43A9-81CC-3AE2DFC5E057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE0F152-CDF7-40F5-9896-195996C61D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="1" activeTab="1" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -886,15 +886,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1001,6 +992,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2055,6 +2052,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -2110,50 +2110,50 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="114">
   <autoFilter ref="A1:O41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="15">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="114"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="113">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="112">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="112">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="111">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="111">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="110">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="110">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="109">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="109">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="108">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="108">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="107">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="107">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="106">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="106">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="105">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="105">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="104">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="104">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="103">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="103">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="102">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="102">
+    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="101">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="101">
+    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="100">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="100">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="99">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2166,46 +2166,46 @@
   <autoFilter ref="A43:O55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="99">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="98">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="98">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="97">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="97">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="96">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="96">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="95">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="95">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="94">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="94">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="93">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="93">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="92">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="92">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="91">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="91">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="90">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="90">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="89">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="89">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="88">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="88">
+    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="87">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="87">
+    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="86">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="86">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="85">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2214,36 +2214,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="84">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="84"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="83">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="83"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="82">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="82">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="81">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="81">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="80">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="80">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="79">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="79">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="78">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="78">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="77">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="77">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="76">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2252,32 +2252,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="75">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="75"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="74">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="74"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="73">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="73">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="72">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="72">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="71">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="71">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="70">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="70">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="69">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="69">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="68">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="68">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="67">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2286,36 +2286,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="64">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="63">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="63">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="62">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="62">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="61">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="61">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="60">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="60">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="59">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="59">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="58">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="58">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="57">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2324,44 +2324,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AB42" totalsRowShown="0" headerRowDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AB42" totalsRowShown="0" headerRowDxfId="56">
   <autoFilter ref="A2:AB42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="28">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="56"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="55">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="54">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="54">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="53">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="53">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="52">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="52">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="51">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="51">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="50">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="50">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="49">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="49">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="48">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="48">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="47">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="46">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="45">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="45">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="44">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="44">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="43">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2373,45 +2373,45 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="43">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="42">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="42">
+    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="41">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -12, IF(table_7_1[[#This Row],[hguide]]="CD", -12, IF(table_7_1[[#This Row],[hguide]]="A", -12, IF(table_7_1[[#This Row],[hguide]]="B", -12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="41">
+    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="40">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 13, IF(table_7_1[[#This Row],[hguide]]="CD", 13, IF(table_7_1[[#This Row],[hguide]]="A", 13, IF(table_7_1[[#This Row],[hguide]]="B", 13, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="0">
+    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="39">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -22, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{FCD7272B-07C5-4D80-8B2B-EFDF0948D1A3}" name="range_y1" dataDxfId="40">
+    <tableColumn id="18" xr3:uid="{FCD7272B-07C5-4D80-8B2B-EFDF0948D1A3}" name="range_y1" dataDxfId="38">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 22, IF(table_7_1[[#This Row],[hguide]]="CD", 27, IF(table_7_1[[#This Row],[hguide]]="A", 20, IF(table_7_1[[#This Row],[hguide]]="B", 16, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="39">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="37">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT("--range_x ", table_7_1[[#This Row],[range_x0]], " ", table_7_1[[#This Row],[range_x1]], " --range_y ", table_7_1[[#This Row],[range_y0]], " ", table_7_1[[#This Row],[range_y1]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{862E4B1D-E776-4C82-956F-64077E0EAD63}" name="universal_layout_y_axis_args" dataDxfId="38">
+    <tableColumn id="29" xr3:uid="{862E4B1D-E776-4C82-956F-64077E0EAD63}" name="universal_layout_y_axis_args" dataDxfId="36">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_x_pos ", table_7_1[[#This Row],[range_x1]] - 1, " --universal_layout_y_axis_y_range ", table_7_1[[#This Row],[range_y0]] + 2.5, " ", table_7_1[[#This Row],[range_y1]] - 1.5, " "), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{80C9383B-6A26-4051-B986-65C11BA3AFE0}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="23" xr3:uid="{010D8635-D593-4849-BEA6-27994308E467}" name="universal_layout_x_axis_args" dataDxfId="37">
+    <tableColumn id="23" xr3:uid="{010D8635-D593-4849-BEA6-27994308E467}" name="universal_layout_x_axis_args" dataDxfId="35">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[show_universal_layout_x_axes]], _xlfn.CONCAT(" --universal_layout_x_axis_deletion_y_pos ", table_7_1[[#This Row],[range_y0]] + 1.5, " --universal_layout_x_axis_insertion_y_pos ", table_7_1[[#This Row],[range_y1]] - 0.5, " --universal_layout_x_axis_x_range ", table_7_1[[#This Row],[range_x0]] + 0.5, " ", table_7_1[[#This Row],[range_x1]] - 1.5), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="36">
+    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="34">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 7, IF(table_7_1[[#This Row],[hguide]]="CD", 8, IF(table_7_1[[#This Row],[hguide]]="A", 6, IF(table_7_1[[#This Row],[hguide]]="B", 5, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="1">
+    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="33">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 17, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="35">
+    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="32">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="34">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{C5B2A575-6AC4-403E-AE67-1624B7F60F7E}" name="format"/>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="33">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2420,46 +2420,46 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A44:O60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="29">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="28">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="25">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="24">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="23">
+    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{EADBB7DC-9D40-44C2-8742-A17A0EB899C3}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="22">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="19">
       <calculatedColumnFormula>IF(table_7_2[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="21">
+    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="20">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{8B58B2DF-3EB7-4D4E-A96D-1BED892121E3}" name="format"/>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2468,46 +2468,46 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A62:O64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="15">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="11">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="7">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="9">
+    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="6">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="7">
+    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="4">
       <calculatedColumnFormula>IF(table_7_3[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="6">
+    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="3">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="3">
+    <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2527,25 +2527,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="214">
       <calculatedColumnFormula array="1">IF(table_1[[#This Row],[dsb_type]]="2DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="1DSB", IF(table_1[[#This Row],[strand]]="R1", 67, 46), IF(table_1[[#This Row],[dsb_type]]="2DSBanti", IF(table_1[[#This Row],[strand]]="R1", 66, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="214">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="213">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="213">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="212">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="212">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="211">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="211">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="210">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="210">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="209">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="209">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="208">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2554,38 +2554,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="208">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="207">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="207"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="206">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="206"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="205">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="205">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="204">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="204">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="203">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="203">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="202">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="202">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="201">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="201">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="200">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="200">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="199">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="199">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="198">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="198">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="197">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="197">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="196">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2597,19 +2597,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="196">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="195">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="195">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="194">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="194">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="193">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="193">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="192">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="192">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="191">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2621,41 +2621,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="191"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="190">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="190"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="189">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="188">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="187">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="186">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="185">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="184">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="183">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="182">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="182">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="181">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="181">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="180">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="180">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="179">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="179">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="178">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2664,47 +2664,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="178">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="177">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="177"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="176">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="176"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="175">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="175">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="174">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="174">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="173">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="172">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="171">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="170">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="170">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="169">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="168">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="168">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="167">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="166">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="165">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="165">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="164">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2713,47 +2713,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="163">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="163"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="162">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="162"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="161">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="160">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="160">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="159">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="159">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="158">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="157">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="156">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="156">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="155">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="154">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="154">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="153">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="152">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="152">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="151">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="151">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="150">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2762,38 +2762,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="150">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="149">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="149"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="148">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="147">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="147">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="146">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="146">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="145">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="145">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="144">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="143">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="142">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="142">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="141">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="141">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="140">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="140">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="139">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="139">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="138">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2802,38 +2802,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="138">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="137">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="137"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="136">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="135">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="135">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="134">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="134">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="133">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="133">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="132">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="132">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="131">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="131">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="130">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="130">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="129">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="129">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="128">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="128">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="127">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2842,38 +2842,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="126">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="126"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="125">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="125"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="124">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="124">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="123">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="123">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="122">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="122">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="121">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="121">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="120">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="120">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="119">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="119">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="118">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="118">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="117">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="117">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="116">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="116">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="115">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3247,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5334D33C-3E16-4C4F-BA76-1F06B33FAC0B}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109:D116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26822,7 +26822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>

</xml_diff>